<commit_message>
added pdf cheat-sheet - charts
</commit_message>
<xml_diff>
--- a/monthly_budget.xlsx
+++ b/monthly_budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://weifieldgroup0-my.sharepoint.com/personal/cjones_weifieldgroup_com/Documents/Desktop/Excel_Udemy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="287" documentId="8_{C5B5F0C7-0F4A-434F-A707-AD3DBEF26536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F62D28AE-3DFA-4984-A538-830F576DDE55}"/>
+  <xr:revisionPtr revIDLastSave="288" documentId="8_{C5B5F0C7-0F4A-434F-A707-AD3DBEF26536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D789A548-24DF-4E5A-9325-FB165F833B1A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chart_monthly_budget" sheetId="9" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Bills</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t xml:space="preserve">2025 Monthly Budget </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                   </t>
   </si>
 </sst>
 </file>
@@ -3374,7 +3377,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0C9C8DCC-8790-49D8-9923-3CE78E6131A0}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7017,10 +7020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7297,6 +7300,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:G2"/>

</xml_diff>

<commit_message>
additional worksheets, pie charts
</commit_message>
<xml_diff>
--- a/monthly_budget.xlsx
+++ b/monthly_budget.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://weifieldgroup0-my.sharepoint.com/personal/cjones_weifieldgroup_com/Documents/Desktop/Excel_Udemy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="288" documentId="8_{C5B5F0C7-0F4A-434F-A707-AD3DBEF26536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D789A548-24DF-4E5A-9325-FB165F833B1A}"/>
+  <xr:revisionPtr revIDLastSave="330" documentId="8_{C5B5F0C7-0F4A-434F-A707-AD3DBEF26536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA84B857-4A39-438E-A2E7-875EAFCC299C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chart_monthly_budget" sheetId="9" r:id="rId1"/>
-    <sheet name="monthly_budget" sheetId="1" r:id="rId2"/>
+    <sheet name="pie_jan_budget" sheetId="11" r:id="rId2"/>
+    <sheet name="pie_feb_budget" sheetId="10" r:id="rId3"/>
+    <sheet name="pie_march_budget" sheetId="12" r:id="rId4"/>
+    <sheet name="monthly_budget" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1143,11 +1146,504 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>monthly_budget!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jan-25</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-DFA2-4997-83CA-986A4783A10C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-DFA2-4997-83CA-986A4783A10C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-DFA2-4997-83CA-986A4783A10C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-DFA2-4997-83CA-986A4783A10C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-DFA2-4997-83CA-986A4783A10C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="1"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="95000"/>
+                      <a:alpha val="54000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>monthly_budget!$B$5:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Rent</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Phone</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Credit Cards</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Food</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Candy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>monthly_budget!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1235</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-DFA2-4997-83CA-986A4783A10C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1158,11 +1654,161 @@
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>monthly_budget!$D$4</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Feb-25</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
+      <c:pie3DChart>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1182,76 +1828,276 @@
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-DB8D-4400-A089-48BE74292322}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-DB8D-4400-A089-48BE74292322}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-DB8D-4400-A089-48BE74292322}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-DB8D-4400-A089-48BE74292322}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-DB8D-4400-A089-48BE74292322}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1262,17 +2108,14 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1285,22 +2128,21 @@
             </c:txPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="1"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="1"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
+            <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:leaderLines>
               <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:ln w="9525">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="95000"/>
+                      <a:alpha val="54000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:round/>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
@@ -1358,7 +2200,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A7A4-48BC-9494-8D06A534E5D3}"/>
+              <c16:uniqueId val="{0000000A-DB8D-4400-A089-48BE74292322}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1372,8 +2214,7 @@
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+      </c:pie3DChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1396,12 +2237,11 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1425,17 +2265,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1444,20 +2295,15 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1485,13 +2331,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -1502,20 +2354,59 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
+      <c:pie3DChart>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>monthly_budget!$G$4</c:f>
+              <c:f>monthly_budget!$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Percent</c:v>
+                  <c:v>Mar-25</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1524,77 +2415,329 @@
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-C97E-439E-8C28-DA5E52968311}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-C97E-439E-8C28-DA5E52968311}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-C97E-439E-8C28-DA5E52968311}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-C97E-439E-8C28-DA5E52968311}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-C97E-439E-8C28-DA5E52968311}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:dPt>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="1"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="95000"/>
+                      <a:alpha val="54000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>monthly_budget!$B$5:$B$9</c:f>
@@ -1620,45 +2763,44 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>monthly_budget!$G$5:$G$9</c:f>
+              <c:f>monthly_budget!$E$5:$E$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.60840085993054405</c:v>
+                  <c:v>1246</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.243261121217133E-2</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20456424673391765</c:v>
+                  <c:v>412</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10286092277162229</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1741359351744666E-2</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CFBF-4F00-A20A-DB894E5F18EF}"/>
+              <c16:uniqueId val="{0000000A-C97E-439E-8C28-DA5E52968311}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+      </c:pie3DChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1682,11 +2824,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1710,17 +2851,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1729,16 +2881,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1859,6 +3006,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="294">
   <cs:axisTitle>
@@ -2336,35 +3523,33 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="268">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2372,37 +3557,44 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2421,14 +3613,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2437,49 +3621,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2491,10 +3661,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -2503,16 +3673,17 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -2530,21 +3701,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2563,14 +3731,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2582,14 +3749,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2603,9 +3770,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2619,12 +3785,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -2636,9 +3796,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2653,108 +3813,115 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2766,12 +3933,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2787,7 +3961,6 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2796,9 +3969,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2814,14 +3986,13 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2830,9 +4001,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2844,46 +4014,38 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="268">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2891,37 +4053,44 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2940,14 +4109,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2956,49 +4117,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3010,10 +4157,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -3022,16 +4169,17 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -3049,21 +4197,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3082,14 +4227,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -3101,14 +4245,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -3122,9 +4266,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3138,12 +4281,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -3155,9 +4292,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3172,108 +4309,115 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3285,12 +4429,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3306,7 +4457,6 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3315,9 +4465,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3333,27 +4482,521 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="268">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3363,12 +5006,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3377,7 +5014,40 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0C9C8DCC-8790-49D8-9923-3CE78E6131A0}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{AFC203FD-9B35-4F80-9097-6B006052682E}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{9F6E1621-8748-4371-8803-2A3A02202817}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{48D17BF3-E4F9-4E1C-B947-70017728F5F3}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6444,6 +8114,105 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8664408" cy="6291513"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14E2FE19-73C0-9B29-5771-CB3411E13E3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8664408" cy="6291513"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E69CC53-D9F9-E661-C28A-6467F385B12B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8664408" cy="6291513"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6374CB1-CEB3-8744-5543-82748088BC3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -6649,78 +8418,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/diagram">
           <dgm:relIds xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:dm="rId3" r:lo="rId4" r:qs="rId5" r:cs="rId6"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Chart 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBCC2E9C-6020-F729-688B-F4C5EBCE92E1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Chart 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E13A7760-CC83-6816-AED2-A0D22F4990D3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7022,8 +8719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated workbook print layouts
</commit_message>
<xml_diff>
--- a/monthly_budget.xlsx
+++ b/monthly_budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://weifieldgroup0-my.sharepoint.com/personal/cjones_weifieldgroup_com/Documents/Desktop/Excel_Udemy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="330" documentId="8_{C5B5F0C7-0F4A-434F-A707-AD3DBEF26536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA84B857-4A39-438E-A2E7-875EAFCC299C}"/>
+  <xr:revisionPtr revIDLastSave="457" documentId="8_{C5B5F0C7-0F4A-434F-A707-AD3DBEF26536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23B983BC-89CC-41DD-8D48-6B389335297A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,16 +90,8 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="171" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -114,20 +106,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Candara"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="24"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Candara"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Candara"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Candara"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Candara"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -200,43 +209,44 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="17" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1036,8 +1046,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.25635842633449396"/>
           <c:y val="0.89519675156039569"/>
-          <c:w val="0.48728314733101213"/>
-          <c:h val="4.6264070343651834E-2"/>
+          <c:w val="0.4874523749047498"/>
+          <c:h val="4.6296042987876256E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2889,6 +2899,1397 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1320" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>monthly_budget!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Feb-25</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="1"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="95000"/>
+                      <a:alpha val="54000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>monthly_budget!$B$5:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Rent</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Phone</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Credit Cards</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Food</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Candy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>monthly_budget!$D$5:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A7C7-43F0-934F-D44007A89866}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>monthly_budget!$B$2</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>2025 Monthly Budget </c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.3488720752762336"/>
+          <c:y val="4.6427624007134689E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14275758083431062"/>
+          <c:y val="0.14333884118465937"/>
+          <c:w val="0.82887362483944826"/>
+          <c:h val="0.65086166570648563"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>monthly_budget!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:shade val="51000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="80000">
+                  <a:schemeClr val="accent6">
+                    <a:shade val="93000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:shade val="94000"/>
+                    <a:satMod val="135000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="16200000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront">
+                <a:rot lat="0" lon="0" rev="0"/>
+              </a:camera>
+              <a:lightRig rig="threePt" dir="t">
+                <a:rot lat="0" lon="0" rev="1200000"/>
+              </a:lightRig>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="63500" h="25400"/>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>monthly_budget!$C$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>45658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45689</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45717</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>monthly_budget!$C$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1235</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1246</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6EA5-4381-A8EC-425194B744D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>monthly_budget!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Phone</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:shade val="51000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="80000">
+                  <a:schemeClr val="accent5">
+                    <a:shade val="93000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:shade val="94000"/>
+                    <a:satMod val="135000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="16200000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront">
+                <a:rot lat="0" lon="0" rev="0"/>
+              </a:camera>
+              <a:lightRig rig="threePt" dir="t">
+                <a:rot lat="0" lon="0" rev="1200000"/>
+              </a:lightRig>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="63500" h="25400"/>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>monthly_budget!$C$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>45658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45689</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45717</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>monthly_budget!$C$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>146</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6EA5-4381-A8EC-425194B744D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>monthly_budget!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Credit Cards</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="51000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="80000">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="93000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="94000"/>
+                    <a:satMod val="135000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="16200000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront">
+                <a:rot lat="0" lon="0" rev="0"/>
+              </a:camera>
+              <a:lightRig rig="threePt" dir="t">
+                <a:rot lat="0" lon="0" rev="1200000"/>
+              </a:lightRig>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="63500" h="25400"/>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>monthly_budget!$C$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>45658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45689</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45717</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>monthly_budget!$C$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>412</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6EA5-4381-A8EC-425194B744D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>monthly_budget!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Food</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="51000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="80000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="93000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="94000"/>
+                    <a:satMod val="135000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="16200000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront">
+                <a:rot lat="0" lon="0" rev="0"/>
+              </a:camera>
+              <a:lightRig rig="threePt" dir="t">
+                <a:rot lat="0" lon="0" rev="1200000"/>
+              </a:lightRig>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="63500" h="25400"/>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>monthly_budget!$C$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>45658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45689</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45717</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>monthly_budget!$C$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>225</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6EA5-4381-A8EC-425194B744D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>monthly_budget!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Candy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="51000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="80000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="93000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="94000"/>
+                    <a:satMod val="135000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="16200000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront">
+                <a:rot lat="0" lon="0" rev="0"/>
+              </a:camera>
+              <a:lightRig rig="threePt" dir="t">
+                <a:rot lat="0" lon="0" rev="1200000"/>
+              </a:lightRig>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="63500" h="25400"/>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>monthly_budget!$C$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>45658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45689</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45717</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>monthly_budget!$C$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6EA5-4381-A8EC-425194B744D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="366732127"/>
+        <c:axId val="366732607"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="366732127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="366732607"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="366732607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="366732127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.25635842633449396"/>
+          <c:y val="0.89519675156039569"/>
+          <c:w val="0.48728314733101213"/>
+          <c:h val="4.6264070343651834E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -3046,6 +4447,83 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="294">
   <cs:axisTitle>
@@ -5010,6 +6488,978 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="294">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0C9C8DCC-8790-49D8-9923-3CE78E6131A0}">
   <sheetPr/>
@@ -5017,7 +7467,8 @@
     <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -5028,7 +7479,8 @@
     <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -5039,7 +7491,8 @@
     <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -5050,7 +7503,8 @@
     <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -6322,7 +8776,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{46A34875-8FB4-4179-B276-E26FB7D4F7B2}" type="pres">
-      <dgm:prSet presAssocID="{A6FBA831-E58C-46D6-9A18-E2DF980F5408}" presName="arrow" presStyleLbl="bgShp" presStyleIdx="0" presStyleCnt="1" custLinFactX="-14467" custLinFactY="15659" custLinFactNeighborX="-100000" custLinFactNeighborY="100000"/>
+      <dgm:prSet presAssocID="{A6FBA831-E58C-46D6-9A18-E2DF980F5408}" presName="arrow" presStyleLbl="bgShp" presStyleIdx="0" presStyleCnt="1" custLinFactNeighborX="2043" custLinFactNeighborY="-1745"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{A0B29CD6-D2B8-42F8-B7AB-7360C2C8539E}" type="pres">
@@ -6425,8 +8879,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="4388167" cy="3071812"/>
+          <a:off x="481354" y="0"/>
+          <a:ext cx="4429701" cy="3058763"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -6465,8 +8919,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="142660" y="933277"/>
-          <a:ext cx="1569781" cy="1205256"/>
+          <a:off x="144010" y="929313"/>
+          <a:ext cx="1584639" cy="1200136"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6603,8 +9057,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="201496" y="992113"/>
-        <a:ext cx="1452109" cy="1087584"/>
+        <a:off x="202596" y="987899"/>
+        <a:ext cx="1467467" cy="1082964"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{3BC48A74-372B-4DC9-9CDF-46CBF1AABACE}">
@@ -6614,8 +9068,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1796384" y="933277"/>
-          <a:ext cx="1569781" cy="1205256"/>
+          <a:off x="1813387" y="929313"/>
+          <a:ext cx="1584639" cy="1200136"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6734,8 +9188,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1855220" y="992113"/>
-        <a:ext cx="1452109" cy="1087584"/>
+        <a:off x="1871973" y="987899"/>
+        <a:ext cx="1467467" cy="1082964"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{63EFDB58-0384-4076-8B1E-50722CC9DD29}">
@@ -6745,8 +9199,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3450107" y="933277"/>
-          <a:ext cx="1569781" cy="1205256"/>
+          <a:off x="3482763" y="929313"/>
+          <a:ext cx="1584639" cy="1200136"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6883,8 +9337,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3508943" y="992113"/>
-        <a:ext cx="1452109" cy="1087584"/>
+        <a:off x="3541349" y="987899"/>
+        <a:ext cx="1467467" cy="1082964"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -8083,7 +10537,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8664408" cy="6291513"/>
+    <xdr:ext cx="8661400" cy="6287168"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8216,15 +10670,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>76201</xdr:colOff>
+      <xdr:colOff>47626</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>523280</xdr:rowOff>
+      <xdr:rowOff>513755</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8256,7 +10710,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="828676" y="247651"/>
+          <a:off x="800101" y="247651"/>
           <a:ext cx="828674" cy="466129"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8321,16 +10775,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47623</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>914398</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1152523</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8344,9 +10798,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5657848" y="1095375"/>
-          <a:ext cx="800101" cy="360045"/>
+        <a:xfrm rot="5400000">
+          <a:off x="5638799" y="2552700"/>
+          <a:ext cx="447674" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
           <a:avLst/>
@@ -8389,16 +10843,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>117144</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>91291</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>13608</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8423,6 +10877,70 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>627784</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>48491</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>67542</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>117764</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Chart 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40F3C0D4-3286-97FF-AC20-15D0E9499AC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="8205107" y="5306787"/>
+    <xdr:ext cx="5497285" cy="3633107"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="18" name="Chart 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{547BA8B8-88EF-4E3F-B6B5-D3FF2B6BCB79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8719,286 +11237,303 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="2" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D3" s="6"/>
-      <c r="G3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="10">
         <v>45658</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="10">
         <v>45689</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="10">
         <v>45717</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="12">
         <v>1235</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="12">
         <v>1198</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="12">
         <v>1246</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="13">
         <f>SUM(C5:E5)</f>
         <v>3679</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="14">
         <f>(F5/F10)</f>
         <v>0.60840085993054405</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="15">
         <v>146</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="15">
         <v>146</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="15">
         <v>146</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="13">
         <f t="shared" ref="F6:F9" si="0">SUM(C6:E6)</f>
         <v>438</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="14">
         <f>(F6/F10)</f>
         <v>7.243261121217133E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="15">
         <v>413</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="15">
         <v>412</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="15">
         <v>412</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="13">
         <f t="shared" si="0"/>
         <v>1237</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="14">
         <f>(F7/F10)</f>
         <v>0.20456424673391765</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="15">
         <v>185</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="16">
         <v>212</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="16">
         <v>225</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="13">
         <f t="shared" si="0"/>
         <v>622</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="14">
         <f>(F8/F10)</f>
         <v>0.10286092277162229</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="15">
         <v>24</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="15">
         <v>21</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="15">
         <v>26</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="13">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="14">
         <f>(F9/F10)</f>
         <v>1.1741359351744666E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="15">
         <f>SUM(C5:C9)</f>
         <v>2003</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="15">
         <f t="shared" ref="D10:F10" si="1">SUM(D5:D9)</f>
         <v>1989</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="15">
         <f t="shared" si="1"/>
         <v>2055</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="15">
         <f t="shared" si="1"/>
         <v>6047</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="17">
         <f>SUM(G5:G9)</f>
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="19">
         <f>MIN(C5:C9)</f>
         <v>24</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="19">
         <f>MIN(D5:D9)</f>
         <v>21</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="19">
         <f>MIN(E5:E9)</f>
         <v>26</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="19">
         <f>MIN(F5:F9)</f>
         <v>71</v>
       </c>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="19">
         <f>MAX(C5:C9)</f>
         <v>1235</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="19">
         <f t="shared" ref="D13:F13" si="2">MAX(D5:D9)</f>
         <v>1198</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="19">
         <f t="shared" si="2"/>
         <v>1246</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="19">
         <f t="shared" si="2"/>
         <v>3679</v>
       </c>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="19">
         <f>AVERAGE(C5:C9)</f>
         <v>400.6</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="19">
         <f t="shared" ref="D14:F14" si="3">AVERAGE(D5:D9)</f>
         <v>397.8</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="19">
         <f t="shared" si="3"/>
         <v>411</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="19">
         <f t="shared" si="3"/>
         <v>1209.4000000000001</v>
       </c>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <f>COUNT(C5:C9)</f>
         <v>5</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="6">
         <f t="shared" ref="D15:F15" si="4">COUNT(D5:D9)</f>
         <v>5</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="6">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="6">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
+      <c r="G15" s="6"/>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -9006,10 +11541,16 @@
   <mergeCells count="1">
     <mergeCell ref="B2:G2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.25" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="125" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C2025 Monthly Budget&amp;RChris Jones</oddHeader>
+    <oddFooter>&amp;C&amp;8&amp;Z&amp;F&amp;R&amp;P</oddFooter>
+  </headerFooter>
   <ignoredErrors>
     <ignoredError sqref="C12:C15 D12:D15 E12:E15 C10:E10" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>